<commit_message>
clustering without repeated families, 0 bias and less singlur fits
</commit_message>
<xml_diff>
--- a/results/main/full_results_PGI_cluster.xlsx
+++ b/results/main/full_results_PGI_cluster.xlsx
@@ -971,16 +971,16 @@
         <v>0.352607761273582</v>
       </c>
       <c r="D2" t="n">
-        <v>0.288270654137325</v>
+        <v>0.299080303690987</v>
       </c>
       <c r="E2" t="n">
-        <v>0.416944868409839</v>
+        <v>0.406135218856178</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.00185784422410827</v>
+        <v>0.000775248258722531</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0328250546613557</v>
+        <v>0.0273099273380589</v>
       </c>
     </row>
     <row r="3">
@@ -994,16 +994,16 @@
         <v>0.319582615600608</v>
       </c>
       <c r="D3" t="n">
-        <v>0.253548863235095</v>
+        <v>0.267868576908842</v>
       </c>
       <c r="E3" t="n">
-        <v>0.38561636796612</v>
+        <v>0.371296654292374</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0139921685631113</v>
+        <v>0.00506180723494574</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0336906899824043</v>
+        <v>0.026384713618248</v>
       </c>
     </row>
     <row r="4">
@@ -1017,16 +1017,16 @@
         <v>0.395559365218808</v>
       </c>
       <c r="D4" t="n">
-        <v>0.334444391020797</v>
+        <v>0.340461036846052</v>
       </c>
       <c r="E4" t="n">
-        <v>0.456674339416818</v>
+        <v>0.450657693591563</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0268316121351132</v>
+        <v>0.00415226825526129</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0311811092846991</v>
+        <v>0.0281113920269159</v>
       </c>
     </row>
     <row r="5">
@@ -1040,16 +1040,16 @@
         <v>0.123639364629483</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0450359333455788</v>
+        <v>0.0710304522333187</v>
       </c>
       <c r="E5" t="n">
-        <v>0.202242795913387</v>
+        <v>0.176248277025647</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.00275537952141111</v>
+        <v>0.000388496009111305</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0401037914713795</v>
+        <v>0.0268412818347775</v>
       </c>
     </row>
     <row r="6">
@@ -1063,16 +1063,16 @@
         <v>0.150080646957203</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0711021993266184</v>
+        <v>0.0900371495108961</v>
       </c>
       <c r="E6" t="n">
-        <v>0.229059094587788</v>
+        <v>0.21012414440351</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0163492823924116</v>
+        <v>0.00217168417341075</v>
       </c>
       <c r="G6" t="n">
-        <v>0.040295126342135</v>
+        <v>0.0306344374726056</v>
       </c>
     </row>
     <row r="7">
@@ -1086,16 +1086,16 @@
         <v>0.178160065785628</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0988120408694443</v>
+        <v>0.117153886279363</v>
       </c>
       <c r="E7" t="n">
-        <v>0.257508090701811</v>
+        <v>0.239166245291893</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0300614555580514</v>
+        <v>0.00185427280031239</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0404836861817262</v>
+        <v>0.0311256017889107</v>
       </c>
     </row>
     <row r="8">
@@ -1109,16 +1109,16 @@
         <v>0.167345231899537</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0673031975755322</v>
+        <v>0.099555497515911</v>
       </c>
       <c r="E8" t="n">
-        <v>0.267387266223543</v>
+        <v>0.235134966283164</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.00066641966418439</v>
+        <v>-0.00290590189549675</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0510418542469415</v>
+        <v>0.0345865991753196</v>
       </c>
     </row>
     <row r="9">
@@ -1132,16 +1132,16 @@
         <v>0.200546487073035</v>
       </c>
       <c r="D9" t="n">
-        <v>0.113545332158088</v>
+        <v>0.134562464472543</v>
       </c>
       <c r="E9" t="n">
-        <v>0.287547641987983</v>
+        <v>0.266530509673527</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0161651670890559</v>
+        <v>-0.000511604608115842</v>
       </c>
       <c r="G9" t="n">
-        <v>0.044388344344361</v>
+        <v>0.0336653176533122</v>
       </c>
     </row>
     <row r="10">
@@ -1155,16 +1155,16 @@
         <v>0.216180255891052</v>
       </c>
       <c r="D10" t="n">
-        <v>0.129587183460683</v>
+        <v>0.152041349939701</v>
       </c>
       <c r="E10" t="n">
-        <v>0.302773328321421</v>
+        <v>0.280319161842402</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0286830635049606</v>
+        <v>-0.00161869347737001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0441801389950862</v>
+        <v>0.0327239316078319</v>
       </c>
     </row>
     <row r="11">
@@ -1178,16 +1178,16 @@
         <v>0.231078807434119</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0892191248623518</v>
+        <v>0.0924784741064575</v>
       </c>
       <c r="E11" t="n">
-        <v>0.372938490005887</v>
+        <v>0.369679140761781</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.0266074944082352</v>
+        <v>0.000510943633949725</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0723773890672283</v>
+        <v>0.0707144557794192</v>
       </c>
     </row>
     <row r="12">
@@ -1201,16 +1201,16 @@
         <v>0.25761663867516</v>
       </c>
       <c r="D12" t="n">
-        <v>0.103474039109996</v>
+        <v>0.11277557544517</v>
       </c>
       <c r="E12" t="n">
-        <v>0.411759238240324</v>
+        <v>0.402457701905151</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.00667898685717974</v>
+        <v>0.00285338594647596</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0786441834516144</v>
+        <v>0.0738985016479543</v>
       </c>
     </row>
     <row r="13">
@@ -1224,16 +1224,16 @@
         <v>0.269248916745021</v>
       </c>
       <c r="D13" t="n">
-        <v>0.128746657831843</v>
+        <v>0.130417595978012</v>
       </c>
       <c r="E13" t="n">
-        <v>0.409751175658198</v>
+        <v>0.408080237512029</v>
       </c>
       <c r="F13" t="n">
-        <v>0.00774443111934483</v>
+        <v>0.000890941520288434</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0716848259761109</v>
+        <v>0.0708323065137799</v>
       </c>
     </row>
     <row r="14">
@@ -1247,16 +1247,16 @@
         <v>0.143215455962746</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0812142979778473</v>
+        <v>0.0907027098539146</v>
       </c>
       <c r="E14" t="n">
-        <v>0.205216613947644</v>
+        <v>0.195728202071576</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.000463077223467801</v>
+        <v>0.0014250710635687</v>
       </c>
       <c r="G14" t="n">
-        <v>0.031633243869846</v>
+        <v>0.0267922174024648</v>
       </c>
     </row>
     <row r="15">
@@ -1270,16 +1270,16 @@
         <v>0.14816176016843</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0855625722612015</v>
+        <v>0.0936529159845769</v>
       </c>
       <c r="E15" t="n">
-        <v>0.210760948075659</v>
+        <v>0.202670604352284</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0172748169217524</v>
+        <v>0.000438344882964851</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0319383611771576</v>
+        <v>0.0278106347876804</v>
       </c>
     </row>
     <row r="16">
@@ -1293,16 +1293,16 @@
         <v>0.163984989723715</v>
       </c>
       <c r="D16" t="n">
-        <v>0.100648266501729</v>
+        <v>0.108736083040986</v>
       </c>
       <c r="E16" t="n">
-        <v>0.227321712945702</v>
+        <v>0.219233896406444</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0294107197077769</v>
+        <v>0.000819811316691935</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0323146547050951</v>
+        <v>0.0281882176952698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>